<commit_message>
bind country to self
</commit_message>
<xml_diff>
--- a/data/initial_state_1.xlsx
+++ b/data/initial_state_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakeboersma/School/AI Project/ai-project-post-break/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B64E13-329F-AD41-A2E2-05003533EB21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A8AFD2-6E7B-3E42-A31D-18D733E827CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="460" windowWidth="23620" windowHeight="15460" xr2:uid="{ED844C13-9B21-4E40-B03F-93EF884CFD31}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Country</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>R21'</t>
+  </si>
+  <si>
+    <t>Self?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -424,208 +433,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60B5BFC-574A-244D-8E0C-16B41A28F5E3}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1">
+    <row r="2" spans="1:11" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1">
         <v>100</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>700</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>2000</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
       <c r="F2" s="1">
         <v>0</v>
       </c>
       <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
         <v>110</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
       <c r="I2" s="1">
         <v>0</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
       </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1">
+    <row r="3" spans="1:11" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1">
         <v>50</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>300</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>1200</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
       <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
         <v>75</v>
       </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
       <c r="I3" s="1">
         <v>0</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
       </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1">
+    <row r="4" spans="1:11" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
         <v>25</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>100</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>300</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
         <v>400</v>
       </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
       <c r="I4" s="1">
         <v>0</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
       </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1">
+    <row r="5" spans="1:11" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1">
         <v>30</v>
-      </c>
-      <c r="C5" s="1">
-        <v>200</v>
       </c>
       <c r="D5" s="1">
         <v>200</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
       <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
         <v>82</v>
       </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
       <c r="I5" s="1">
         <v>0</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
       </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1">
+    <row r="6" spans="1:11" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1">
         <v>70</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>500</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>1700</v>
       </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
       <c r="F6" s="1">
         <v>0</v>
       </c>
       <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
         <v>71</v>
       </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
       <c r="I6" s="1">
         <v>0</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
       </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1"/>
-    <row r="8" spans="1:10" s="1" customFormat="1"/>
+    <row r="7" spans="1:11" s="1" customFormat="1"/>
+    <row r="8" spans="1:11" s="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
depth bound, max frontier size, and version of anytime
</commit_message>
<xml_diff>
--- a/data/initial_state_1.xlsx
+++ b/data/initial_state_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakeboersma/School/AI Project/ai-project-post-break/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B9A712-613C-1E4A-8DDB-3A5DFA0E469A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE5862A-831C-A64B-9484-2D14DD1D7BD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="1060" windowWidth="23620" windowHeight="15460" xr2:uid="{ED844C13-9B21-4E40-B03F-93EF884CFD31}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -520,13 +520,13 @@
         <v>17</v>
       </c>
       <c r="C3" s="1">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="E3" s="1">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -590,13 +590,13 @@
         <v>17</v>
       </c>
       <c r="C5" s="1">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1">
-        <v>700</v>
+        <v>550</v>
       </c>
       <c r="E5" s="1">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>

</xml_diff>